<commit_message>
Implemented sonar selection function. Added pins used to pinlist
</commit_message>
<xml_diff>
--- a/pin_list.xlsx
+++ b/pin_list.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>Team Goose, MAVRIC TM4C1294XL Pin listing</t>
   </si>
@@ -65,10 +65,25 @@
     <t>TIMER_4 CCP0 (Sonar event capture)</t>
   </si>
   <si>
+    <t>GPIO (Sonar analog/power mux enable)</t>
+  </si>
+  <si>
     <t>I2C_0 SCL (RPi)</t>
   </si>
   <si>
     <t>I2C_0 SDA (RPi)</t>
+  </si>
+  <si>
+    <t>GPIO (Sonar digital mux enable)</t>
+  </si>
+  <si>
+    <t>GPIO (Sonar mux select 0)</t>
+  </si>
+  <si>
+    <t>GPIO (Sonar mux select 1)</t>
+  </si>
+  <si>
+    <t>GPIO (Sonar mux select 2)</t>
   </si>
   <si>
     <t>C</t>
@@ -259,7 +274,7 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Good" xfId="20" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Good" xfId="20" builtinId="54" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -332,7 +347,7 @@
   <dimension ref="B1:J22"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -343,11 +358,12 @@
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.8582995951417"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="34"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.2874493927125"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.1457489878542"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="29.7287449392713"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="24.251012145749"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.5748987854251"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.1417004048583"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.5748987854251"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.8178137651822"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="23.080971659919"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="16.165991902834"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.5748987854251"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -430,114 +446,129 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>15</v>
       </c>
+      <c r="D7" s="0" t="s">
+        <v>16</v>
+      </c>
       <c r="E7" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="I7" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="J7" s="0" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="0" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="0" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="0" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed pin assignments for some motor and sonar pins. Updated pinlist
</commit_message>
<xml_diff>
--- a/pin_list.xlsx
+++ b/pin_list.xlsx
@@ -62,76 +62,76 @@
     <t>B</t>
   </si>
   <si>
+    <t>GPIO (Sonar analog/power mux enable)</t>
+  </si>
+  <si>
+    <t>I2C_0 SCL (RPi)</t>
+  </si>
+  <si>
+    <t>I2C_0 SDA (RPi)</t>
+  </si>
+  <si>
+    <t>GPIO (Sonar digital mux enable)</t>
+  </si>
+  <si>
+    <t>GPIO (Sonar mux select 0)</t>
+  </si>
+  <si>
+    <t>GPIO (Sonar mux select 1)</t>
+  </si>
+  <si>
+    <t>GPIO (Sonar mux select 2)</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>PWM_0 Gen_1 Out_0 (Left motor)</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>PWM_0 Gen_2 Out_0 (Right motor)</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>GPIO (Left motor IN_A)</t>
+  </si>
+  <si>
+    <t>GPIO (Left motor IN_B)</t>
+  </si>
+  <si>
+    <t>GPIO (Right motor IN_A)</t>
+  </si>
+  <si>
     <t>TIMER_4 CCP0 (Sonar event capture)</t>
-  </si>
-  <si>
-    <t>GPIO (Sonar analog/power mux enable)</t>
-  </si>
-  <si>
-    <t>I2C_0 SCL (RPi)</t>
-  </si>
-  <si>
-    <t>I2C_0 SDA (RPi)</t>
-  </si>
-  <si>
-    <t>GPIO (Sonar digital mux enable)</t>
-  </si>
-  <si>
-    <t>GPIO (Sonar mux select 0)</t>
-  </si>
-  <si>
-    <t>GPIO (Sonar mux select 1)</t>
-  </si>
-  <si>
-    <t>GPIO (Sonar mux select 2)</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>PWM_0 Gen_1 Out_0 (Left motor)</t>
-  </si>
-  <si>
-    <t>G</t>
-  </si>
-  <si>
-    <t>PWM_0 Gen_2 Out_0 (Right motor)</t>
-  </si>
-  <si>
-    <t>H</t>
-  </si>
-  <si>
-    <t>I</t>
-  </si>
-  <si>
-    <t>J</t>
-  </si>
-  <si>
-    <t>K</t>
-  </si>
-  <si>
-    <t>L</t>
-  </si>
-  <si>
-    <t>M</t>
-  </si>
-  <si>
-    <t>GPIO (Left motor IN_A)</t>
-  </si>
-  <si>
-    <t>GPIO (Left motor IN_B)</t>
-  </si>
-  <si>
-    <t>GPIO (Right motor IN_A)</t>
   </si>
   <si>
     <t>GPIO (Right motor IN_B)</t>
@@ -274,7 +274,7 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Good" xfId="20" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Good" xfId="20" builtinId="54" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -346,8 +346,8 @@
   </sheetPr>
   <dimension ref="B1:J22"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G18" activeCellId="0" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -450,104 +450,104 @@
       <c r="B7" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="D7" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="E7" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="0" t="s">
+      <c r="F7" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="0" t="s">
+      <c r="G7" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="G7" s="0" t="s">
+      <c r="H7" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="H7" s="0" t="s">
+      <c r="I7" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="I7" s="0" t="s">
+      <c r="J7" s="0" t="s">
         <v>21</v>
-      </c>
-      <c r="J7" s="0" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="0" t="s">
         <v>26</v>
-      </c>
-      <c r="E11" s="0" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="0" t="s">
         <v>28</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="0" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="0" t="s">
+      <c r="C18" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="0" t="s">
+      <c r="D18" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="D18" s="0" t="s">
+      <c r="E18" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="E18" s="0" t="s">
+      <c r="G18" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="G18" s="0" t="s">
+      <c r="H18" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="H18" s="0" t="s">
+      <c r="J18" s="0" t="s">
         <v>40</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Tested digital mux circuit for sonar echo pulse. No longer using analog mux. Distance is now reported as 999 cm for unresponsive sonar
</commit_message>
<xml_diff>
--- a/pin_list.xlsx
+++ b/pin_list.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>Team Goose, MAVRIC TM4C1294XL Pin listing</t>
   </si>
@@ -62,9 +62,6 @@
     <t>B</t>
   </si>
   <si>
-    <t>GPIO (Sonar analog/power mux enable)</t>
-  </si>
-  <si>
     <t>I2C_0 SCL (RPi)</t>
   </si>
   <si>
@@ -74,6 +71,39 @@
     <t>GPIO (Sonar digital mux enable)</t>
   </si>
   <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>PWM_0 Gen_1 Out_0 (Left motor)</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>PWM_0 Gen_2 Out_0 (Right motor)</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
     <t>GPIO (Sonar mux select 0)</t>
   </si>
   <si>
@@ -81,39 +111,6 @@
   </si>
   <si>
     <t>GPIO (Sonar mux select 2)</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>PWM_0 Gen_1 Out_0 (Left motor)</t>
-  </si>
-  <si>
-    <t>G</t>
-  </si>
-  <si>
-    <t>PWM_0 Gen_2 Out_0 (Right motor)</t>
-  </si>
-  <si>
-    <t>H</t>
-  </si>
-  <si>
-    <t>I</t>
-  </si>
-  <si>
-    <t>J</t>
-  </si>
-  <si>
-    <t>K</t>
   </si>
   <si>
     <t>L</t>
@@ -274,7 +271,7 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Good" xfId="20" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="20" builtinId="54" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -346,20 +343,20 @@
   </sheetPr>
   <dimension ref="B1:J22"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G18" activeCellId="0" sqref="G18"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H7" activeCellId="0" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.5748987854251"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.995951417004"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.4291497975708"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.8582995951417"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="34"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.2874493927125"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="29.7287449392713"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="24.251012145749"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.080971659919"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.251012145749"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.2064777327935"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.5182186234818"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.9919028340081"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="34.5991902834008"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.8178137651822"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="23.080971659919"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="16.165991902834"/>
@@ -450,125 +447,122 @@
       <c r="B7" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="E7" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="0" t="s">
+      <c r="F7" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="0" t="s">
+      <c r="G7" s="0" t="s">
         <v>17</v>
-      </c>
-      <c r="G7" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="H7" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="I7" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="J7" s="0" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="E16" s="0" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="0" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="0" t="s">
+      <c r="D18" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="D18" s="0" t="s">
+      <c r="E18" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="E18" s="0" t="s">
+      <c r="G18" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="G18" s="0" t="s">
+      <c r="H18" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="H18" s="0" t="s">
+      <c r="J18" s="0" t="s">
         <v>39</v>
-      </c>
-      <c r="J18" s="0" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="0" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated to reflect master
</commit_message>
<xml_diff>
--- a/pin_list.xlsx
+++ b/pin_list.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>Team Goose, MAVRIC TM4C1294XL Pin listing</t>
   </si>
@@ -62,9 +62,6 @@
     <t>B</t>
   </si>
   <si>
-    <t>GPIO (Sonar analog/power mux enable)</t>
-  </si>
-  <si>
     <t>I2C_0 SCL (RPi)</t>
   </si>
   <si>
@@ -74,6 +71,39 @@
     <t>GPIO (Sonar digital mux enable)</t>
   </si>
   <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>PWM_0 Gen_1 Out_0 (Left motor)</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>PWM_0 Gen_2 Out_0 (Right motor)</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
     <t>GPIO (Sonar mux select 0)</t>
   </si>
   <si>
@@ -81,39 +111,6 @@
   </si>
   <si>
     <t>GPIO (Sonar mux select 2)</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>PWM_0 Gen_1 Out_0 (Left motor)</t>
-  </si>
-  <si>
-    <t>G</t>
-  </si>
-  <si>
-    <t>PWM_0 Gen_2 Out_0 (Right motor)</t>
-  </si>
-  <si>
-    <t>H</t>
-  </si>
-  <si>
-    <t>I</t>
-  </si>
-  <si>
-    <t>J</t>
-  </si>
-  <si>
-    <t>K</t>
   </si>
   <si>
     <t>L</t>
@@ -274,7 +271,7 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Good" xfId="20" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="20" builtinId="54" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -346,20 +343,20 @@
   </sheetPr>
   <dimension ref="B1:J22"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G18" activeCellId="0" sqref="G18"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H7" activeCellId="0" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.5748987854251"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.995951417004"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.4291497975708"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.8582995951417"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="34"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.2874493927125"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="29.7287449392713"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="24.251012145749"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.080971659919"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.251012145749"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.2064777327935"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.5182186234818"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.9919028340081"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="34.5991902834008"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.8178137651822"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="23.080971659919"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="16.165991902834"/>
@@ -450,125 +447,122 @@
       <c r="B7" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="E7" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="0" t="s">
+      <c r="F7" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="0" t="s">
+      <c r="G7" s="0" t="s">
         <v>17</v>
-      </c>
-      <c r="G7" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="H7" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="I7" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="J7" s="0" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="E16" s="0" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="0" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="0" t="s">
+      <c r="D18" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="D18" s="0" t="s">
+      <c r="E18" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="E18" s="0" t="s">
+      <c r="G18" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="G18" s="0" t="s">
+      <c r="H18" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="H18" s="0" t="s">
+      <c r="J18" s="0" t="s">
         <v>39</v>
-      </c>
-      <c r="J18" s="0" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="0" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
3/11/2015 Brandon. Motor controls (kinda).
</commit_message>
<xml_diff>
--- a/pin_list.xlsx
+++ b/pin_list.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="13665" windowHeight="2925"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="125725" iterateDelta="1E-4"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>Team Goose, MAVRIC TM4C1294XL Pin listing</t>
   </si>
@@ -95,9 +95,6 @@
     <t>F</t>
   </si>
   <si>
-    <t>PWM_0 Gen_1 Out_0 (Left motor)</t>
-  </si>
-  <si>
     <t>G</t>
   </si>
   <si>
@@ -150,37 +147,28 @@
   </si>
   <si>
     <t>Q</t>
+  </si>
+  <si>
+    <t>Left Motor Speed Detection (input)</t>
+  </si>
+  <si>
+    <t>Right Motor Speed Detection (input)</t>
+  </si>
+  <si>
+    <t>`</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
-  </numFmts>
-  <fonts count="6">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="11"/>
@@ -190,7 +178,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -213,7 +201,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -221,61 +209,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="7">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Good" xfId="20" builtinId="54" customBuiltin="true"/>
+  <cellStyles count="2">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="TableStyleLight1" xfId="1"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -334,253 +285,542 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
   <dimension ref="B1:J22"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G18" activeCellId="0" sqref="G18"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.5748987854251"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.995951417004"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.4291497975708"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.8582995951417"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="34"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.2874493927125"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="29.7287449392713"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="24.251012145749"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.8178137651822"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="23.080971659919"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="16.165991902834"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.5748987854251"/>
+    <col min="1" max="1" width="8.5703125"/>
+    <col min="2" max="2" width="11"/>
+    <col min="3" max="3" width="31.42578125"/>
+    <col min="4" max="4" width="32.85546875"/>
+    <col min="5" max="5" width="34"/>
+    <col min="6" max="6" width="26.28515625"/>
+    <col min="7" max="7" width="29.7109375"/>
+    <col min="8" max="8" width="24.28515625"/>
+    <col min="9" max="9" width="22.85546875"/>
+    <col min="10" max="10" width="23.140625"/>
+    <col min="11" max="11" width="16.140625"/>
+    <col min="12" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="2:10">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C4" s="2" t="s">
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+    </row>
+    <row r="2" spans="2:10">
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+    </row>
+    <row r="3" spans="2:10">
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+    </row>
+    <row r="4" spans="2:10">
+      <c r="C4" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="3" t="s">
+    <row r="5" spans="2:10">
+      <c r="B5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="I5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J5" s="3" t="s">
+      <c r="J5" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="0" t="s">
+    <row r="6" spans="2:10">
+      <c r="B6" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="0" t="s">
+    <row r="7" spans="2:10">
+      <c r="B7" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="0" t="s">
+      <c r="E7" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="0" t="s">
+      <c r="F7" t="s">
         <v>17</v>
       </c>
-      <c r="G7" s="0" t="s">
+      <c r="G7" t="s">
         <v>18</v>
       </c>
-      <c r="H7" s="0" t="s">
+      <c r="H7" t="s">
         <v>19</v>
       </c>
-      <c r="I7" s="0" t="s">
+      <c r="I7" t="s">
         <v>20</v>
       </c>
-      <c r="J7" s="0" t="s">
+      <c r="J7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="0" t="s">
+    <row r="8" spans="2:10">
+      <c r="B8" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="0" t="s">
+    <row r="9" spans="2:10">
+      <c r="B9" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="0" t="s">
+    <row r="10" spans="2:10">
+      <c r="B10" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="0" t="s">
+      <c r="C10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10">
+      <c r="B11" t="s">
         <v>25</v>
       </c>
-      <c r="E11" s="0" t="s">
+      <c r="E11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10">
+      <c r="B12" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="0" t="s">
+      <c r="C12" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="0" t="s">
+    </row>
+    <row r="13" spans="2:10">
+      <c r="B13" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="0" t="s">
+    <row r="14" spans="2:10">
+      <c r="B14" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="0" t="s">
+    <row r="15" spans="2:10">
+      <c r="B15" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="0" t="s">
+    <row r="16" spans="2:10">
+      <c r="B16" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="0" t="s">
+    <row r="17" spans="2:10">
+      <c r="B17" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="0" t="s">
+    <row r="18" spans="2:10">
+      <c r="B18" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="0" t="s">
+      <c r="C18" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="0" t="s">
+      <c r="D18" t="s">
         <v>35</v>
       </c>
-      <c r="D18" s="0" t="s">
+      <c r="E18" t="s">
         <v>36</v>
       </c>
-      <c r="E18" s="0" t="s">
+      <c r="G18" t="s">
         <v>37</v>
       </c>
-      <c r="G18" s="0" t="s">
+      <c r="H18" t="s">
         <v>38</v>
       </c>
-      <c r="H18" s="0" t="s">
+      <c r="J18" t="s">
         <v>39</v>
       </c>
-      <c r="J18" s="0" t="s">
+    </row>
+    <row r="19" spans="2:10">
+      <c r="B19" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="0" t="s">
+    <row r="20" spans="2:10">
+      <c r="B20" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="0" t="s">
+    <row r="21" spans="2:10">
+      <c r="B21" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="0" t="s">
+    <row r="22" spans="2:10">
+      <c r="B22" t="s">
         <v>43</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="0" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:J3"/>
   </mergeCells>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>